<commit_message>
started exploratory data analysis part
</commit_message>
<xml_diff>
--- a/assets/data/news.xlsx
+++ b/assets/data/news.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21029"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3FEA018-913D-4875-9A32-8961F1C6C730}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9EEE16C-D62F-49CC-971F-31E4AF84179F}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="70">
   <si>
     <t>Kurt Cobain</t>
   </si>
@@ -134,6 +134,102 @@
   </si>
   <si>
     <t>BBC Article Regarding new TV series, that looks at Joan Crawford and Bette Davis’ legendary hatred for each other</t>
+  </si>
+  <si>
+    <t>Dr. Seuss</t>
+  </si>
+  <si>
+    <t>2/3</t>
+  </si>
+  <si>
+    <t>Dr. Seuss Birthday</t>
+  </si>
+  <si>
+    <t>https://keepincalendar.com/March-2/Dr.%20Seuss%20Day/61</t>
+  </si>
+  <si>
+    <t>Rosetta Stone</t>
+  </si>
+  <si>
+    <t>18/3</t>
+  </si>
+  <si>
+    <t>Rosetta Stone is laying off 17 percent of its workforce</t>
+  </si>
+  <si>
+    <t>https://www.bizjournals.com/washington/blog/techflash/2016/03/rosetta-stone-is-laying-off-17-percent-of-its.html</t>
+  </si>
+  <si>
+    <t>Albert Einstein</t>
+  </si>
+  <si>
+    <t>14/3</t>
+  </si>
+  <si>
+    <t>http://ncsm.gov.in/born-on-march-14-you-share-your-birthday-with-albert-einstein/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">J. K. Rowling </t>
+  </si>
+  <si>
+    <t>29/3</t>
+  </si>
+  <si>
+    <t>Famours Tweet</t>
+  </si>
+  <si>
+    <t>https://twitter.com/jk_rowling/status/847012362360180736?lang=en</t>
+  </si>
+  <si>
+    <t> Date for Floyd Mayweather vs. Conor McGregor</t>
+  </si>
+  <si>
+    <t>Floyd Mayweather Jr.</t>
+  </si>
+  <si>
+    <t>12/3</t>
+  </si>
+  <si>
+    <t>https://www.flocombat.com/articles/5062516-las-vegas-venue-holds-date-for-floyd-mayweather-vs-conor-mcgregor</t>
+  </si>
+  <si>
+    <t>North Korea's sixth nuclear test</t>
+  </si>
+  <si>
+    <t>13/4</t>
+  </si>
+  <si>
+    <t>North Korea</t>
+  </si>
+  <si>
+    <t>https://www.cnbc.com/2017/04/13/north-koreas-sixth-nuclear-test.html</t>
+  </si>
+  <si>
+    <t>Chemical Attack in Syria</t>
+  </si>
+  <si>
+    <t>https://www.diplomatie.gouv.fr/en/country-files/syria/events/article/chemical-attack-in-syria-4-april-2017-follow-the-reactions-of-france</t>
+  </si>
+  <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>USA</t>
+  </si>
+  <si>
+    <t>Jamaica</t>
+  </si>
+  <si>
+    <t>UK</t>
+  </si>
+  <si>
+    <t>Switzerland</t>
+  </si>
+  <si>
+    <t>Germany</t>
+  </si>
+  <si>
+    <t>Syria</t>
   </si>
 </sst>
 </file>
@@ -181,9 +277,7 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -465,21 +559,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A4:D19"/>
+  <dimension ref="A4:E49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="32.28515625" customWidth="1"/>
     <col min="2" max="2" width="21.85546875" customWidth="1"/>
-    <col min="3" max="3" width="32.5703125" customWidth="1"/>
-    <col min="4" max="4" width="65" customWidth="1"/>
+    <col min="3" max="3" width="54" customWidth="1"/>
+    <col min="4" max="4" width="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -490,10 +584,13 @@
         <v>4</v>
       </c>
       <c r="D4" t="s">
+        <v>63</v>
+      </c>
+      <c r="E4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>0</v>
       </c>
@@ -504,10 +601,13 @@
         <v>6</v>
       </c>
       <c r="D5" t="s">
+        <v>64</v>
+      </c>
+      <c r="E5" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -518,10 +618,13 @@
         <v>10</v>
       </c>
       <c r="D6" t="s">
+        <v>64</v>
+      </c>
+      <c r="E6" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -532,10 +635,13 @@
         <v>6</v>
       </c>
       <c r="D7" t="s">
+        <v>65</v>
+      </c>
+      <c r="E7" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>17</v>
       </c>
@@ -546,10 +652,13 @@
         <v>16</v>
       </c>
       <c r="D8" t="s">
+        <v>64</v>
+      </c>
+      <c r="E8" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>18</v>
       </c>
@@ -560,10 +669,13 @@
         <v>20</v>
       </c>
       <c r="D9" t="s">
+        <v>64</v>
+      </c>
+      <c r="E9" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>22</v>
       </c>
@@ -574,10 +686,13 @@
         <v>25</v>
       </c>
       <c r="D10" t="s">
+        <v>64</v>
+      </c>
+      <c r="E10" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>28</v>
       </c>
@@ -588,24 +703,30 @@
         <v>27</v>
       </c>
       <c r="D11" t="s">
+        <v>66</v>
+      </c>
+      <c r="E11" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>30</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="C12" t="s">
         <v>32</v>
       </c>
       <c r="D12" t="s">
+        <v>67</v>
+      </c>
+      <c r="E12" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>35</v>
       </c>
@@ -616,32 +737,225 @@
         <v>37</v>
       </c>
       <c r="D13" t="s">
+        <v>64</v>
+      </c>
+      <c r="E13" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B14" s="1"/>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B15" s="1"/>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B16" s="1"/>
-    </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B17" s="1"/>
-    </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B18" s="1"/>
-    </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B19" s="1"/>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>38</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C14" t="s">
+        <v>40</v>
+      </c>
+      <c r="D14" t="s">
+        <v>64</v>
+      </c>
+      <c r="E14" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>42</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C15" t="s">
+        <v>44</v>
+      </c>
+      <c r="D15" t="s">
+        <v>64</v>
+      </c>
+      <c r="E15" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>46</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C16" t="s">
+        <v>6</v>
+      </c>
+      <c r="D16" t="s">
+        <v>68</v>
+      </c>
+      <c r="E16" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>49</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C17" t="s">
+        <v>51</v>
+      </c>
+      <c r="D17" t="s">
+        <v>66</v>
+      </c>
+      <c r="E17" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>54</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C18" t="s">
+        <v>53</v>
+      </c>
+      <c r="D18" t="s">
+        <v>64</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>59</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C19" t="s">
+        <v>57</v>
+      </c>
+      <c r="D19" t="s">
+        <v>59</v>
+      </c>
+      <c r="E19" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>69</v>
+      </c>
+      <c r="B20" s="1">
+        <v>43285</v>
+      </c>
+      <c r="C20" t="s">
+        <v>61</v>
+      </c>
+      <c r="D20" t="s">
+        <v>69</v>
+      </c>
+      <c r="E20" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B21" s="1"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B22" s="1"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B23" s="1"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B24" s="1"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B25" s="1"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B26" s="1"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B27" s="1"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B28" s="1"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B29" s="1"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B30" s="1"/>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B31" s="1"/>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B32" s="1"/>
+    </row>
+    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B33" s="1"/>
+    </row>
+    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B34" s="1"/>
+    </row>
+    <row r="35" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B35" s="1"/>
+    </row>
+    <row r="36" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B36" s="1"/>
+    </row>
+    <row r="37" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B37" s="1"/>
+    </row>
+    <row r="38" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B38" s="1"/>
+    </row>
+    <row r="39" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B39" s="1"/>
+    </row>
+    <row r="40" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B40" s="1"/>
+    </row>
+    <row r="41" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B41" s="1"/>
+    </row>
+    <row r="42" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B42" s="1"/>
+    </row>
+    <row r="43" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B43" s="1"/>
+    </row>
+    <row r="44" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B44" s="1"/>
+    </row>
+    <row r="45" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B45" s="1"/>
+    </row>
+    <row r="46" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B46" s="1"/>
+    </row>
+    <row r="47" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B47" s="1"/>
+    </row>
+    <row r="48" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B48" s="1"/>
+    </row>
+    <row r="49" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B49" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C12" r:id="rId1" display="http://www.internationaldisabilityalliance.org/wdsd-2017-gva" xr:uid="{66948650-B453-404E-8E4E-EC844C2DCAFE}"/>
+    <hyperlink ref="E9" r:id="rId1" xr:uid="{2621BD01-B8CC-47D7-8E8C-98AB6DAA26AE}"/>
+    <hyperlink ref="E8" r:id="rId2" xr:uid="{AE9AE635-72BF-4AAD-A205-58F83C437C36}"/>
+    <hyperlink ref="E18" r:id="rId3" xr:uid="{763D8046-F5D3-4E24-A92C-E7C3DB0AD238}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>